<commit_message>
Gui with button and png
</commit_message>
<xml_diff>
--- a/coordinates.xlsx
+++ b/coordinates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fergg\PycharmProjects\Weather.App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D30E3EE8-B033-4B29-BA59-7D051A19E01C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099B3267-863E-4B90-A25E-B4CB3B8F7B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="585" windowWidth="13125" windowHeight="11700" xr2:uid="{1DA58168-CD36-4793-B84D-8D6DF031218A}"/>
+    <workbookView xWindow="51060" yWindow="1170" windowWidth="13125" windowHeight="11700" xr2:uid="{1DA58168-CD36-4793-B84D-8D6DF031218A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,33 +71,18 @@
     <t>oxford</t>
   </si>
   <si>
-    <t>catdiff bute park</t>
-  </si>
-  <si>
-    <t>ross-on-wye</t>
-  </si>
-  <si>
     <t>aberporth</t>
   </si>
   <si>
     <t>cwmystwyth</t>
   </si>
   <si>
-    <t>cambridge niab</t>
-  </si>
-  <si>
     <t>lowestoft</t>
   </si>
   <si>
     <t>shawbury</t>
   </si>
   <si>
-    <t>suntton bonington</t>
-  </si>
-  <si>
-    <t>waddinton</t>
-  </si>
-  <si>
     <t>sheffield</t>
   </si>
   <si>
@@ -113,9 +98,6 @@
     <t>whitby</t>
   </si>
   <si>
-    <t>newton rigg</t>
-  </si>
-  <si>
     <t>durham</t>
   </si>
   <si>
@@ -131,22 +113,40 @@
     <t>dunstaffnage</t>
   </si>
   <si>
-    <t>tiree</t>
-  </si>
-  <si>
     <t>braemar</t>
   </si>
   <si>
-    <t>stornoway airport</t>
-  </si>
-  <si>
-    <t>wick airport</t>
-  </si>
-  <si>
-    <t>ballypatrick forest</t>
-  </si>
-  <si>
     <t>armagh</t>
+  </si>
+  <si>
+    <t>ballypatrick</t>
+  </si>
+  <si>
+    <t>stornoway</t>
+  </si>
+  <si>
+    <t>cambridge</t>
+  </si>
+  <si>
+    <t>newtonrigg</t>
+  </si>
+  <si>
+    <t>cardiff</t>
+  </si>
+  <si>
+    <t>rossonwye</t>
+  </si>
+  <si>
+    <t>waddington</t>
+  </si>
+  <si>
+    <t>suttonbonington</t>
+  </si>
+  <si>
+    <t>iree</t>
+  </si>
+  <si>
+    <t>wickairpor</t>
   </si>
 </sst>
 </file>
@@ -502,10 +502,13 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -619,7 +622,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B11">
         <v>0.52</v>
@@ -630,7 +633,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>0.62</v>
@@ -641,7 +644,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>0.48</v>
@@ -652,7 +655,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>0.53</v>
@@ -663,7 +666,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>0.82</v>
@@ -674,7 +677,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -685,7 +688,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>0.61</v>
@@ -696,7 +699,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1">
         <v>0.71</v>
@@ -707,7 +710,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1">
         <v>0.84</v>
@@ -718,7 +721,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1">
         <v>0.71</v>
@@ -729,7 +732,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1">
         <v>0.51</v>
@@ -740,7 +743,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1">
         <v>0.68</v>
@@ -751,7 +754,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1">
         <v>0.71</v>
@@ -762,7 +765,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1">
         <v>0.79</v>
@@ -773,7 +776,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>0.65</v>
@@ -784,7 +787,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B26" s="1">
         <v>0.81</v>
@@ -795,7 +798,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B27" s="1">
         <v>0.65</v>
@@ -806,7 +809,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1">
         <v>0.5</v>
@@ -817,7 +820,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B29" s="1">
         <v>0.79</v>
@@ -828,7 +831,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1">
         <v>0.48</v>
@@ -839,7 +842,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1">
         <v>0.45</v>
@@ -850,7 +853,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B32" s="1">
         <v>0.74</v>
@@ -861,7 +864,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B33" s="1">
         <v>0.5</v>
@@ -872,7 +875,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1">
         <v>0.73</v>
@@ -883,7 +886,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B35" s="1">
         <v>0.43</v>
@@ -894,7 +897,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B36" s="1">
         <v>0.39</v>

</xml_diff>